<commit_message>
modify intellij idea keymaps.xlsx
</commit_message>
<xml_diff>
--- a/IntelliJ_IDEA/Intellij IDEA keymaps.xlsx
+++ b/IntelliJ_IDEA/Intellij IDEA keymaps.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="290">
   <si>
     <t>编辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1155,6 +1155,34 @@
   </si>
   <si>
     <t>Ctrl + M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ctrl + Shift + T</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新建Test测试类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ctrl + Shift + C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复制类文件的地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重构Field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ctrl + Alt + C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重构Constant</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1250,10 +1278,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1596,7 +1624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1607,7 +1635,7 @@
   <dimension ref="A1:L144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1624,28 +1652,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1753,10 +1781,10 @@
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="3" t="s">
         <v>148</v>
       </c>
@@ -1841,10 +1869,10 @@
       <c r="F9" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:12" ht="12" customHeight="1">
       <c r="A10" s="3" t="s">
@@ -1873,10 +1901,10 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="14.1" customHeight="1">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -2047,10 +2075,10 @@
       <c r="F17" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="12" customHeight="1">
       <c r="A18" s="3" t="s">
@@ -2187,10 +2215,10 @@
       <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>111</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -2311,10 +2339,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="12" customHeight="1">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2337,10 +2365,10 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="12" customHeight="1">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2355,10 +2383,10 @@
       <c r="F29" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="H29" s="7"/>
+      <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8" ht="12" customHeight="1">
       <c r="A30" s="3" t="s">
@@ -2373,10 +2401,10 @@
       <c r="D30" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="3" t="s">
         <v>263</v>
       </c>
@@ -2497,10 +2525,10 @@
         <v>133</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="F35" s="8"/>
       <c r="G35" s="3" t="s">
         <v>273</v>
       </c>
@@ -2557,7 +2585,12 @@
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="B38" s="1"/>
+      <c r="A38" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>284</v>
+      </c>
       <c r="C38" s="3" t="s">
         <v>138</v>
       </c>
@@ -2566,13 +2599,28 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="B39" s="1"/>
+      <c r="A39" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="B40" s="1"/>
+      <c r="A40" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="B41" s="1"/>
+      <c r="A41" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="B42" s="1"/>
@@ -2924,22 +2972,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="H1" s="7"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="12" customHeight="1">
       <c r="A2" s="3" t="s">
@@ -3053,10 +3101,10 @@
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="7"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="3" t="s">
         <v>148</v>
       </c>
@@ -3141,10 +3189,10 @@
       <c r="F9" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:12" ht="12" customHeight="1">
       <c r="A10" s="3" t="s">
@@ -3335,20 +3383,20 @@
       <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D17" s="7"/>
+      <c r="D17" s="8"/>
       <c r="E17" s="3" t="s">
         <v>170</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
@@ -3655,10 +3703,10 @@
       <c r="F29" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="H29" s="7"/>
+      <c r="H29" s="8"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
@@ -3667,14 +3715,14 @@
       <c r="B30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7" t="s">
+      <c r="D30" s="8"/>
+      <c r="E30" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="8"/>
       <c r="G30" s="3" t="s">
         <v>263</v>
       </c>
@@ -3767,10 +3815,10 @@
       <c r="B34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="D34" s="7"/>
+      <c r="D34" s="8"/>
       <c r="E34" s="3" t="s">
         <v>203</v>
       </c>
@@ -3797,10 +3845,10 @@
       <c r="D35" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="F35" s="8"/>
       <c r="G35" s="3" t="s">
         <v>273</v>
       </c>
@@ -4179,12 +4227,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="G17:H17"/>
@@ -4192,6 +4234,12 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="C34:D34"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>